<commit_message>
Working on note 10
</commit_message>
<xml_diff>
--- a/resources/analysis/char distribution/Character Distribution.xlsx
+++ b/resources/analysis/char distribution/Character Distribution.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\mzatt\Projects\Git - v4j\resources\analysis\char distribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC67E23F-F2E8-4046-A55F-01ACAF1CB16A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2E1EDC-0B97-4BA4-9D24-9EF0218CD65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13320" yWindow="120" windowWidth="15405" windowHeight="15450" tabRatio="806" xr2:uid="{ECC3CD32-09AE-4AED-9EE9-BD1FB4BEAB7F}"/>
+    <workbookView xWindow="10575" yWindow="15" windowWidth="15630" windowHeight="15585" tabRatio="806" activeTab="2" xr2:uid="{ECC3CD32-09AE-4AED-9EE9-BD1FB4BEAB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Compact" sheetId="2" r:id="rId1"/>
     <sheet name="TwoSamplesCharDistributionTest" sheetId="4" r:id="rId2"/>
     <sheet name="CountCharactersByCluster" sheetId="3" r:id="rId3"/>
-    <sheet name="Compact (2)" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2377" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="622">
   <si>
     <t>Transcription     : AUGMENTED</t>
   </si>
@@ -1544,12 +1543,6 @@
   </si>
   <si>
     <t>+ (389 / 694) (35.92% / 32.12%)</t>
-  </si>
-  <si>
-    <t>First word of paragraph VS. standard population</t>
-  </si>
-  <si>
-    <t>*INITIALS* of First word of paragraph VS. standard population</t>
   </si>
   <si>
     <t>Too few samples</t>
@@ -2413,259 +2406,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="84">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="48">
     <dxf>
       <fill>
         <patternFill>
@@ -3317,8 +3058,8 @@
   </sheetPr>
   <dimension ref="A1:AI58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:AD49"/>
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6836,7 +6577,7 @@
         <v>43</v>
       </c>
       <c r="E57" s="23" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="F57" s="22"/>
       <c r="G57" s="22"/>
@@ -7188,7 +6929,7 @@
   <dimension ref="A1:AG49"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:AC49"/>
+      <selection activeCell="U36" sqref="U36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7393,7 +7134,7 @@
         <v>386</v>
       </c>
       <c r="N9" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="O9" t="s">
         <v>387</v>
@@ -7411,7 +7152,7 @@
         <v>391</v>
       </c>
       <c r="T9" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="U9" t="s">
         <v>392</v>
@@ -7426,7 +7167,7 @@
         <v>395</v>
       </c>
       <c r="Y9" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="Z9" t="s">
         <v>396</v>
@@ -7473,28 +7214,28 @@
         <v>50</v>
       </c>
       <c r="J10" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="K10" t="s">
         <v>51</v>
       </c>
       <c r="L10" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="M10" t="s">
         <v>52</v>
       </c>
       <c r="N10" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="O10" t="s">
         <v>53</v>
       </c>
       <c r="P10" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="Q10" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="R10" t="s">
         <v>54</v>
@@ -7503,7 +7244,7 @@
         <v>55</v>
       </c>
       <c r="T10" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="U10" t="s">
         <v>56</v>
@@ -7512,7 +7253,7 @@
         <v>57</v>
       </c>
       <c r="W10" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="X10" t="s">
         <v>58</v>
@@ -7524,7 +7265,7 @@
         <v>59</v>
       </c>
       <c r="AA10" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="AB10" t="s">
         <v>60</v>
@@ -7577,16 +7318,16 @@
         <v>71</v>
       </c>
       <c r="N11" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="O11" t="s">
         <v>72</v>
       </c>
       <c r="P11" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="Q11" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="R11" t="s">
         <v>73</v>
@@ -7595,7 +7336,7 @@
         <v>74</v>
       </c>
       <c r="T11" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="U11" t="s">
         <v>75</v>
@@ -7610,7 +7351,7 @@
         <v>78</v>
       </c>
       <c r="Y11" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="Z11" t="s">
         <v>79</v>
@@ -7657,28 +7398,28 @@
         <v>88</v>
       </c>
       <c r="J12" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="K12" t="s">
         <v>89</v>
       </c>
       <c r="L12" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="M12" t="s">
         <v>90</v>
       </c>
       <c r="N12" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="O12" t="s">
         <v>91</v>
       </c>
       <c r="P12" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="Q12" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="R12" t="s">
         <v>92</v>
@@ -7687,7 +7428,7 @@
         <v>93</v>
       </c>
       <c r="T12" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="U12" t="s">
         <v>94</v>
@@ -7696,19 +7437,19 @@
         <v>95</v>
       </c>
       <c r="W12" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="X12" t="s">
         <v>96</v>
       </c>
       <c r="Y12" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="Z12" t="s">
         <v>97</v>
       </c>
       <c r="AA12" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="AB12" t="s">
         <v>98</v>
@@ -7749,7 +7490,7 @@
         <v>105</v>
       </c>
       <c r="J13" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="K13" t="s">
         <v>106</v>
@@ -7761,16 +7502,16 @@
         <v>108</v>
       </c>
       <c r="N13" t="s">
+        <v>496</v>
+      </c>
+      <c r="O13" t="s">
+        <v>497</v>
+      </c>
+      <c r="P13" t="s">
         <v>498</v>
       </c>
-      <c r="O13" t="s">
+      <c r="Q13" t="s">
         <v>499</v>
-      </c>
-      <c r="P13" t="s">
-        <v>500</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>501</v>
       </c>
       <c r="R13" t="s">
         <v>109</v>
@@ -7779,7 +7520,7 @@
         <v>110</v>
       </c>
       <c r="T13" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="U13" t="s">
         <v>111</v>
@@ -7794,7 +7535,7 @@
         <v>114</v>
       </c>
       <c r="Y13" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="Z13" t="s">
         <v>115</v>
@@ -7988,7 +7729,7 @@
         <v>409</v>
       </c>
       <c r="N18" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="O18" t="s">
         <v>410</v>
@@ -8021,7 +7762,7 @@
         <v>419</v>
       </c>
       <c r="Y18" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="Z18" t="s">
         <v>420</v>
@@ -8063,7 +7804,7 @@
         <v>124</v>
       </c>
       <c r="J19" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="K19" t="s">
         <v>125</v>
@@ -8075,13 +7816,13 @@
         <v>127</v>
       </c>
       <c r="N19" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="O19" t="s">
         <v>128</v>
       </c>
       <c r="P19" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="Q19" t="s">
         <v>129</v>
@@ -8093,7 +7834,7 @@
         <v>131</v>
       </c>
       <c r="T19" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="U19" t="s">
         <v>132</v>
@@ -8161,13 +7902,13 @@
         <v>149</v>
       </c>
       <c r="N20" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="O20" t="s">
         <v>150</v>
       </c>
       <c r="P20" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="Q20" t="s">
         <v>151</v>
@@ -8179,7 +7920,7 @@
         <v>153</v>
       </c>
       <c r="T20" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="U20" t="s">
         <v>154</v>
@@ -8194,7 +7935,7 @@
         <v>157</v>
       </c>
       <c r="Y20" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="Z20" t="s">
         <v>158</v>
@@ -8235,7 +7976,7 @@
         <v>167</v>
       </c>
       <c r="J21" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="K21" t="s">
         <v>168</v>
@@ -8247,13 +7988,13 @@
         <v>170</v>
       </c>
       <c r="N21" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="O21" t="s">
         <v>171</v>
       </c>
       <c r="P21" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="Q21" t="s">
         <v>172</v>
@@ -8265,7 +8006,7 @@
         <v>174</v>
       </c>
       <c r="T21" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="U21" t="s">
         <v>175</v>
@@ -8280,7 +8021,7 @@
         <v>178</v>
       </c>
       <c r="Y21" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="Z21" t="s">
         <v>179</v>
@@ -8333,7 +8074,7 @@
         <v>192</v>
       </c>
       <c r="N22" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="O22" t="s">
         <v>193</v>
@@ -8366,7 +8107,7 @@
         <v>202</v>
       </c>
       <c r="Y22" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="Z22" t="s">
         <v>203</v>
@@ -8538,7 +8279,7 @@
         <v>433</v>
       </c>
       <c r="N27" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="O27" t="s">
         <v>434</v>
@@ -8556,7 +8297,7 @@
         <v>438</v>
       </c>
       <c r="T27" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="U27" t="s">
         <v>439</v>
@@ -8571,7 +8312,7 @@
         <v>442</v>
       </c>
       <c r="Y27" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="Z27" t="s">
         <v>443</v>
@@ -8613,7 +8354,7 @@
         <v>212</v>
       </c>
       <c r="J28" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="K28" t="s">
         <v>213</v>
@@ -8625,13 +8366,13 @@
         <v>215</v>
       </c>
       <c r="N28" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="O28" t="s">
         <v>216</v>
       </c>
       <c r="P28" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="Q28" t="s">
         <v>217</v>
@@ -8643,7 +8384,7 @@
         <v>219</v>
       </c>
       <c r="T28" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="U28" t="s">
         <v>220</v>
@@ -8652,7 +8393,7 @@
         <v>221</v>
       </c>
       <c r="W28" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="X28" t="s">
         <v>222</v>
@@ -8711,13 +8452,13 @@
         <v>236</v>
       </c>
       <c r="N29" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="O29" t="s">
         <v>237</v>
       </c>
       <c r="P29" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="Q29" t="s">
         <v>238</v>
@@ -8729,7 +8470,7 @@
         <v>240</v>
       </c>
       <c r="T29" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="U29" t="s">
         <v>241</v>
@@ -8744,7 +8485,7 @@
         <v>244</v>
       </c>
       <c r="Y29" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="Z29" t="s">
         <v>245</v>
@@ -8785,7 +8526,7 @@
         <v>254</v>
       </c>
       <c r="J30" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K30" t="s">
         <v>255</v>
@@ -8797,13 +8538,13 @@
         <v>257</v>
       </c>
       <c r="N30" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="O30" t="s">
         <v>258</v>
       </c>
       <c r="P30" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="Q30" t="s">
         <v>259</v>
@@ -8815,7 +8556,7 @@
         <v>261</v>
       </c>
       <c r="T30" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="U30" t="s">
         <v>262</v>
@@ -8830,13 +8571,13 @@
         <v>265</v>
       </c>
       <c r="Y30" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="Z30" t="s">
         <v>266</v>
       </c>
       <c r="AA30" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="AB30" t="s">
         <v>267</v>
@@ -8883,7 +8624,7 @@
         <v>278</v>
       </c>
       <c r="N31" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="O31" t="s">
         <v>279</v>
@@ -8916,7 +8657,7 @@
         <v>288</v>
       </c>
       <c r="Y31" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="Z31" t="s">
         <v>289</v>
@@ -9076,7 +8817,7 @@
         <v>452</v>
       </c>
       <c r="J36" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="K36" t="s">
         <v>453</v>
@@ -9088,25 +8829,25 @@
         <v>455</v>
       </c>
       <c r="N36" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="O36" t="s">
         <v>456</v>
       </c>
       <c r="P36" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="Q36" t="s">
         <v>457</v>
       </c>
       <c r="R36" t="s">
+        <v>541</v>
+      </c>
+      <c r="S36" t="s">
+        <v>542</v>
+      </c>
+      <c r="T36" t="s">
         <v>543</v>
-      </c>
-      <c r="S36" t="s">
-        <v>544</v>
-      </c>
-      <c r="T36" t="s">
-        <v>545</v>
       </c>
       <c r="U36" t="s">
         <v>458</v>
@@ -9121,13 +8862,13 @@
         <v>43</v>
       </c>
       <c r="Y36" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="Z36" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="AA36" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="AB36" t="s">
         <v>460</v>
@@ -9145,52 +8886,52 @@
         <v>292</v>
       </c>
       <c r="D37" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="E37" t="s">
         <v>293</v>
       </c>
       <c r="F37" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="G37" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="H37" t="s">
         <v>294</v>
       </c>
       <c r="I37" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="J37" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="K37" t="s">
         <v>295</v>
       </c>
       <c r="L37" t="s">
+        <v>548</v>
+      </c>
+      <c r="M37" t="s">
+        <v>549</v>
+      </c>
+      <c r="N37" t="s">
         <v>550</v>
       </c>
-      <c r="M37" t="s">
+      <c r="O37" t="s">
         <v>551</v>
       </c>
-      <c r="N37" t="s">
+      <c r="P37" t="s">
         <v>552</v>
       </c>
-      <c r="O37" t="s">
+      <c r="Q37" t="s">
         <v>553</v>
       </c>
-      <c r="P37" t="s">
+      <c r="R37" t="s">
         <v>554</v>
       </c>
-      <c r="Q37" t="s">
+      <c r="S37" t="s">
         <v>555</v>
-      </c>
-      <c r="R37" t="s">
-        <v>556</v>
-      </c>
-      <c r="S37" t="s">
-        <v>557</v>
       </c>
       <c r="T37" t="s">
         <v>43</v>
@@ -9231,7 +8972,7 @@
         <v>299</v>
       </c>
       <c r="D38" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="E38" t="s">
         <v>300</v>
@@ -9240,7 +8981,7 @@
         <v>301</v>
       </c>
       <c r="G38" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="H38" t="s">
         <v>302</v>
@@ -9249,37 +8990,37 @@
         <v>303</v>
       </c>
       <c r="J38" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="K38" t="s">
         <v>304</v>
       </c>
       <c r="L38" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="M38" t="s">
         <v>305</v>
       </c>
       <c r="N38" t="s">
+        <v>560</v>
+      </c>
+      <c r="O38" t="s">
+        <v>561</v>
+      </c>
+      <c r="P38" t="s">
         <v>562</v>
       </c>
-      <c r="O38" t="s">
+      <c r="Q38" t="s">
         <v>563</v>
       </c>
-      <c r="P38" t="s">
+      <c r="R38" t="s">
+        <v>560</v>
+      </c>
+      <c r="S38" t="s">
         <v>564</v>
       </c>
-      <c r="Q38" t="s">
-        <v>565</v>
-      </c>
-      <c r="R38" t="s">
-        <v>562</v>
-      </c>
-      <c r="S38" t="s">
-        <v>566</v>
-      </c>
       <c r="T38" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="U38" t="s">
         <v>306</v>
@@ -9300,7 +9041,7 @@
         <v>43</v>
       </c>
       <c r="AA38" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="AB38" t="s">
         <v>308</v>
@@ -9335,37 +9076,37 @@
         <v>315</v>
       </c>
       <c r="J39" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="K39" t="s">
         <v>316</v>
       </c>
       <c r="L39" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="M39" t="s">
         <v>317</v>
       </c>
       <c r="N39" t="s">
+        <v>567</v>
+      </c>
+      <c r="O39" t="s">
+        <v>568</v>
+      </c>
+      <c r="P39" t="s">
         <v>569</v>
       </c>
-      <c r="O39" t="s">
+      <c r="Q39" t="s">
         <v>570</v>
       </c>
-      <c r="P39" t="s">
+      <c r="R39" t="s">
         <v>571</v>
       </c>
-      <c r="Q39" t="s">
+      <c r="S39" t="s">
         <v>572</v>
       </c>
-      <c r="R39" t="s">
+      <c r="T39" t="s">
         <v>573</v>
-      </c>
-      <c r="S39" t="s">
-        <v>574</v>
-      </c>
-      <c r="T39" t="s">
-        <v>575</v>
       </c>
       <c r="U39" t="s">
         <v>318</v>
@@ -9386,7 +9127,7 @@
         <v>43</v>
       </c>
       <c r="AA39" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="AB39" t="s">
         <v>320</v>
@@ -9421,7 +9162,7 @@
         <v>327</v>
       </c>
       <c r="J40" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="K40" t="s">
         <v>328</v>
@@ -9433,25 +9174,25 @@
         <v>330</v>
       </c>
       <c r="N40" t="s">
+        <v>575</v>
+      </c>
+      <c r="O40" t="s">
+        <v>576</v>
+      </c>
+      <c r="P40" t="s">
         <v>577</v>
       </c>
-      <c r="O40" t="s">
+      <c r="Q40" t="s">
         <v>578</v>
       </c>
-      <c r="P40" t="s">
+      <c r="R40" t="s">
         <v>579</v>
       </c>
-      <c r="Q40" t="s">
+      <c r="S40" t="s">
         <v>580</v>
       </c>
-      <c r="R40" t="s">
+      <c r="T40" t="s">
         <v>581</v>
-      </c>
-      <c r="S40" t="s">
-        <v>582</v>
-      </c>
-      <c r="T40" t="s">
-        <v>583</v>
       </c>
       <c r="U40" t="s">
         <v>331</v>
@@ -9463,7 +9204,7 @@
         <v>43</v>
       </c>
       <c r="X40" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="Y40" t="s">
         <v>43</v>
@@ -9472,7 +9213,7 @@
         <v>43</v>
       </c>
       <c r="AA40" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="AB40" t="s">
         <v>333</v>
@@ -9620,52 +9361,52 @@
         <v>464</v>
       </c>
       <c r="H45" t="s">
+        <v>582</v>
+      </c>
+      <c r="I45" t="s">
+        <v>583</v>
+      </c>
+      <c r="J45" t="s">
         <v>584</v>
       </c>
-      <c r="I45" t="s">
+      <c r="K45" t="s">
         <v>585</v>
       </c>
-      <c r="J45" t="s">
+      <c r="L45" t="s">
         <v>586</v>
       </c>
-      <c r="K45" t="s">
+      <c r="M45" t="s">
         <v>587</v>
       </c>
-      <c r="L45" t="s">
+      <c r="N45" t="s">
+        <v>43</v>
+      </c>
+      <c r="O45" t="s">
+        <v>584</v>
+      </c>
+      <c r="P45" t="s">
         <v>588</v>
       </c>
-      <c r="M45" t="s">
+      <c r="Q45" t="s">
         <v>589</v>
       </c>
-      <c r="N45" t="s">
-        <v>43</v>
-      </c>
-      <c r="O45" t="s">
-        <v>586</v>
-      </c>
-      <c r="P45" t="s">
+      <c r="R45" t="s">
         <v>590</v>
       </c>
-      <c r="Q45" t="s">
+      <c r="S45" t="s">
         <v>591</v>
       </c>
-      <c r="R45" t="s">
-        <v>592</v>
-      </c>
-      <c r="S45" t="s">
-        <v>593</v>
-      </c>
       <c r="T45" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="U45" t="s">
         <v>465</v>
       </c>
       <c r="V45" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="W45" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="X45" t="s">
         <v>43</v>
@@ -9695,10 +9436,10 @@
         <v>43</v>
       </c>
       <c r="D46" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E46" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="F46" t="s">
         <v>334</v>
@@ -9707,40 +9448,40 @@
         <v>335</v>
       </c>
       <c r="H46" t="s">
+        <v>595</v>
+      </c>
+      <c r="I46" t="s">
+        <v>596</v>
+      </c>
+      <c r="J46" t="s">
+        <v>43</v>
+      </c>
+      <c r="K46" t="s">
         <v>597</v>
       </c>
-      <c r="I46" t="s">
+      <c r="L46" t="s">
+        <v>595</v>
+      </c>
+      <c r="M46" t="s">
+        <v>43</v>
+      </c>
+      <c r="N46" t="s">
+        <v>43</v>
+      </c>
+      <c r="O46" t="s">
+        <v>43</v>
+      </c>
+      <c r="P46" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>43</v>
+      </c>
+      <c r="R46" t="s">
         <v>598</v>
       </c>
-      <c r="J46" t="s">
-        <v>43</v>
-      </c>
-      <c r="K46" t="s">
-        <v>599</v>
-      </c>
-      <c r="L46" t="s">
-        <v>597</v>
-      </c>
-      <c r="M46" t="s">
-        <v>43</v>
-      </c>
-      <c r="N46" t="s">
-        <v>43</v>
-      </c>
-      <c r="O46" t="s">
-        <v>43</v>
-      </c>
-      <c r="P46" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>43</v>
-      </c>
-      <c r="R46" t="s">
-        <v>600</v>
-      </c>
       <c r="S46" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="T46" t="s">
         <v>43</v>
@@ -9749,10 +9490,10 @@
         <v>336</v>
       </c>
       <c r="V46" t="s">
+        <v>596</v>
+      </c>
+      <c r="W46" t="s">
         <v>598</v>
-      </c>
-      <c r="W46" t="s">
-        <v>600</v>
       </c>
       <c r="X46" t="s">
         <v>43</v>
@@ -9764,7 +9505,7 @@
         <v>337</v>
       </c>
       <c r="AA46" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="AB46" t="s">
         <v>338</v>
@@ -9781,7 +9522,7 @@
         <v>43</v>
       </c>
       <c r="D47" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="E47" t="s">
         <v>339</v>
@@ -9793,40 +9534,40 @@
         <v>341</v>
       </c>
       <c r="H47" t="s">
+        <v>601</v>
+      </c>
+      <c r="I47" t="s">
+        <v>602</v>
+      </c>
+      <c r="J47" t="s">
         <v>603</v>
       </c>
-      <c r="I47" t="s">
+      <c r="K47" t="s">
         <v>604</v>
       </c>
-      <c r="J47" t="s">
+      <c r="L47" t="s">
         <v>605</v>
       </c>
-      <c r="K47" t="s">
+      <c r="M47" t="s">
         <v>606</v>
       </c>
-      <c r="L47" t="s">
+      <c r="N47" t="s">
+        <v>43</v>
+      </c>
+      <c r="O47" t="s">
+        <v>601</v>
+      </c>
+      <c r="P47" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>43</v>
+      </c>
+      <c r="R47" t="s">
         <v>607</v>
       </c>
-      <c r="M47" t="s">
-        <v>608</v>
-      </c>
-      <c r="N47" t="s">
-        <v>43</v>
-      </c>
-      <c r="O47" t="s">
-        <v>603</v>
-      </c>
-      <c r="P47" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>43</v>
-      </c>
-      <c r="R47" t="s">
-        <v>609</v>
-      </c>
       <c r="S47" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="T47" t="s">
         <v>43</v>
@@ -9835,7 +9576,7 @@
         <v>342</v>
       </c>
       <c r="V47" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="W47" t="s">
         <v>43</v>
@@ -9850,7 +9591,7 @@
         <v>343</v>
       </c>
       <c r="AA47" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="AB47" t="s">
         <v>344</v>
@@ -9864,7 +9605,7 @@
         <v>0</v>
       </c>
       <c r="C48" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="D48" t="s">
         <v>345</v>
@@ -9879,40 +9620,40 @@
         <v>348</v>
       </c>
       <c r="H48" t="s">
+        <v>610</v>
+      </c>
+      <c r="I48" t="s">
+        <v>610</v>
+      </c>
+      <c r="J48" t="s">
+        <v>43</v>
+      </c>
+      <c r="K48" t="s">
+        <v>611</v>
+      </c>
+      <c r="L48" t="s">
+        <v>610</v>
+      </c>
+      <c r="M48" t="s">
         <v>612</v>
       </c>
-      <c r="I48" t="s">
+      <c r="N48" t="s">
+        <v>43</v>
+      </c>
+      <c r="O48" t="s">
+        <v>609</v>
+      </c>
+      <c r="P48" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>43</v>
+      </c>
+      <c r="R48" t="s">
+        <v>610</v>
+      </c>
+      <c r="S48" t="s">
         <v>612</v>
-      </c>
-      <c r="J48" t="s">
-        <v>43</v>
-      </c>
-      <c r="K48" t="s">
-        <v>613</v>
-      </c>
-      <c r="L48" t="s">
-        <v>612</v>
-      </c>
-      <c r="M48" t="s">
-        <v>614</v>
-      </c>
-      <c r="N48" t="s">
-        <v>43</v>
-      </c>
-      <c r="O48" t="s">
-        <v>611</v>
-      </c>
-      <c r="P48" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q48" t="s">
-        <v>43</v>
-      </c>
-      <c r="R48" t="s">
-        <v>612</v>
-      </c>
-      <c r="S48" t="s">
-        <v>614</v>
       </c>
       <c r="T48" t="s">
         <v>43</v>
@@ -9921,7 +9662,7 @@
         <v>349</v>
       </c>
       <c r="V48" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="W48" t="s">
         <v>43</v>
@@ -9936,7 +9677,7 @@
         <v>350</v>
       </c>
       <c r="AA48" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="AB48" t="s">
         <v>351</v>
@@ -9965,49 +9706,49 @@
         <v>355</v>
       </c>
       <c r="H49" t="s">
+        <v>614</v>
+      </c>
+      <c r="I49" t="s">
+        <v>615</v>
+      </c>
+      <c r="J49" t="s">
+        <v>615</v>
+      </c>
+      <c r="K49" t="s">
         <v>616</v>
       </c>
-      <c r="I49" t="s">
+      <c r="L49" t="s">
         <v>617</v>
       </c>
-      <c r="J49" t="s">
-        <v>617</v>
-      </c>
-      <c r="K49" t="s">
+      <c r="M49" t="s">
         <v>618</v>
       </c>
-      <c r="L49" t="s">
+      <c r="N49" t="s">
+        <v>43</v>
+      </c>
+      <c r="O49" t="s">
+        <v>43</v>
+      </c>
+      <c r="P49" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>43</v>
+      </c>
+      <c r="R49" t="s">
         <v>619</v>
       </c>
-      <c r="M49" t="s">
+      <c r="S49" t="s">
         <v>620</v>
       </c>
-      <c r="N49" t="s">
-        <v>43</v>
-      </c>
-      <c r="O49" t="s">
-        <v>43</v>
-      </c>
-      <c r="P49" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q49" t="s">
-        <v>43</v>
-      </c>
-      <c r="R49" t="s">
-        <v>621</v>
-      </c>
-      <c r="S49" t="s">
-        <v>622</v>
-      </c>
       <c r="T49" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="U49" t="s">
         <v>356</v>
       </c>
       <c r="V49" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="W49" t="s">
         <v>43</v>
@@ -10323,7 +10064,7 @@
   </sheetPr>
   <dimension ref="A1:AJ23"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
@@ -11326,2543 +11067,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDEE8D32-CC71-4848-B2FD-4F2C60145E58}">
-  <sheetPr>
-    <tabColor rgb="FFFF0000"/>
-  </sheetPr>
-  <dimension ref="A1:AI38"/>
-  <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J47" sqref="J47"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="23"/>
-    <col min="2" max="2" width="9" style="33" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="14" hidden="1" customWidth="1"/>
-    <col min="4" max="11" width="3.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="3.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="2.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="2.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="3.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="3.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="3.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="2.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="3.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.140625" style="23"/>
-    <col min="31" max="31" width="3.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="55.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="33" max="35" width="9.140625" style="23"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B1" s="33" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:35" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21"/>
-      <c r="B3" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="M3" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="O3" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="P3" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q3" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="R3" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="S3" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="T3" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="U3" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="V3" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="W3" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="X3" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y3" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z3" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA3" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB3" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC3" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="AD3" s="21"/>
-      <c r="AG3" s="21"/>
-      <c r="AH3" s="21"/>
-      <c r="AI3" s="21"/>
-    </row>
-    <row r="4" spans="1:35" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="29">
-        <v>0</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="I4" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="J4" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="K4" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="M4" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="N4" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="O4" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="P4" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="Q4" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="R4" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="S4" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="T4" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="U4" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="V4" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="W4" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="X4" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="Y4" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Z4" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AA4" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AB4" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AC4" s="17" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B5" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="30">
-        <v>0</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>361</v>
-      </c>
-      <c r="K5" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="N5" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="O5" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="P5" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q5" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="R5" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="S5" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="T5" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="U5" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="V5" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="W5" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="X5" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Y5" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="Z5" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AA5" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AB5" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AC5" s="17" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B6" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="30">
-        <v>0</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>361</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="I6" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="J6" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="L6" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="M6" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="N6" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="O6" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="P6" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q6" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="R6" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="S6" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="T6" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="U6" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="V6" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="W6" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="X6" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="Y6" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Z6" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AA6" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AB6" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AC6" s="17" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B7" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="30">
-        <v>0</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>361</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="K7" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="L7" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="M7" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="N7" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="O7" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="P7" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q7" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="R7" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="S7" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="T7" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="U7" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="V7" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="W7" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="X7" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="Y7" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Z7" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AA7" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="AB7" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AC7" s="17" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="31">
-        <v>0</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>361</v>
-      </c>
-      <c r="J8" s="18" t="s">
-        <v>361</v>
-      </c>
-      <c r="K8" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="L8" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="M8" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="N8" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="O8" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="P8" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="Q8" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="R8" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="S8" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="T8" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="U8" s="18" t="s">
-        <v>364</v>
-      </c>
-      <c r="V8" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="W8" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="X8" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="Y8" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="Z8" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="AA8" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="AB8" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="AC8" s="19" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="9" spans="1:35" s="23" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="34"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="22"/>
-      <c r="S9" s="22"/>
-      <c r="T9" s="22"/>
-      <c r="U9" s="22"/>
-      <c r="V9" s="22"/>
-      <c r="W9" s="22"/>
-      <c r="X9" s="22"/>
-      <c r="Y9" s="22"/>
-      <c r="Z9" s="22"/>
-      <c r="AA9" s="22"/>
-      <c r="AB9" s="22"/>
-      <c r="AC9" s="22"/>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B11" s="33" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="12" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="K13" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="L13" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="M13" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="N13" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="O13" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="P13" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q13" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="R13" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="S13" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="T13" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="U13" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="V13" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="W13" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="X13" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y13" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z13" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA13" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB13" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC13" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="AD13" s="21"/>
-    </row>
-    <row r="14" spans="1:35" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="29">
-        <v>0</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="J14" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="K14" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="L14" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="M14" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="N14" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="O14" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="P14" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q14" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="R14" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="S14" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="T14" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="U14" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="V14" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="W14" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="X14" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Y14" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z14" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AA14" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB14" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AC14" s="17" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B15" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="30">
-        <v>1.5E-3</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="I15" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="J15" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="K15" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="L15" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="M15" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="N15" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="O15" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="P15" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q15" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="R15" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="S15" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="T15" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="U15" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="V15" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="W15" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="X15" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Y15" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Z15" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AA15" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AB15" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AC15" s="17" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B16" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="30">
-        <v>0</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="I16" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="J16" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="K16" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="L16" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="M16" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="N16" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="O16" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="P16" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q16" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="R16" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="S16" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="T16" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="U16" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="V16" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="W16" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="X16" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Y16" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Z16" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AA16" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AB16" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AC16" s="17" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="17" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B17" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="30">
-        <v>0</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="H17" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="I17" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="J17" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="K17" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="L17" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="M17" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="N17" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="O17" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="P17" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q17" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="R17" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="S17" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="T17" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="U17" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="V17" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="W17" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="X17" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Y17" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Z17" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AA17" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AB17" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AC17" s="17" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="18" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="31">
-        <v>0</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="G18" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="H18" s="18" t="s">
-        <v>364</v>
-      </c>
-      <c r="I18" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="J18" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="K18" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="L18" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="M18" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="N18" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O18" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="P18" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q18" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="R18" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="S18" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="T18" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="U18" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="V18" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="W18" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="X18" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="Y18" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z18" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="AA18" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB18" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="AC18" s="19" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="19" spans="2:29" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="34"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="22"/>
-      <c r="S19" s="22"/>
-      <c r="T19" s="22"/>
-      <c r="U19" s="22"/>
-      <c r="V19" s="22"/>
-      <c r="W19" s="22"/>
-      <c r="X19" s="22"/>
-      <c r="Y19" s="22"/>
-      <c r="Z19" s="22"/>
-      <c r="AA19" s="22"/>
-      <c r="AB19" s="22"/>
-      <c r="AC19" s="22"/>
-    </row>
-    <row r="20" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B20" s="33" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="21" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="G22" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="H22" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="I22" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="J22" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="K22" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="L22" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="M22" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="N22" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="O22" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="P22" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q22" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="R22" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="S22" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="T22" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="U22" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="V22" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="W22" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="X22" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y22" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z22" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA22" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB22" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC22" s="26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="2:29" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="29">
-        <v>0</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="H23" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="I23" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="J23" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="K23" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="L23" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="M23" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="N23" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="O23" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="P23" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="Q23" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="R23" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="S23" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="T23" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="U23" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="V23" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="W23" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="X23" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="Y23" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Z23" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AA23" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AB23" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AC23" s="17" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="24" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B24" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="30">
-        <v>0</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="H24" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="I24" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="J24" s="16" t="s">
-        <v>361</v>
-      </c>
-      <c r="K24" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="L24" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="M24" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="N24" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="O24" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="P24" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q24" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="R24" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="S24" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="T24" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="U24" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="V24" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="W24" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="X24" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Y24" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="Z24" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AA24" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AB24" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AC24" s="17" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="25" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B25" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="30">
-        <v>0</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>361</v>
-      </c>
-      <c r="G25" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="H25" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="I25" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="J25" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="K25" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="L25" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="M25" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="N25" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="O25" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="P25" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q25" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="R25" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="S25" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="T25" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="U25" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="V25" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="W25" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="X25" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="Y25" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Z25" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AA25" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AB25" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AC25" s="17" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="26" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B26" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="30">
-        <v>0</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="H26" s="16" t="s">
-        <v>361</v>
-      </c>
-      <c r="I26" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="J26" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="K26" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="L26" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="M26" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="N26" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="O26" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="P26" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q26" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="R26" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="S26" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="T26" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="U26" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="V26" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="W26" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="X26" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="Y26" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Z26" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AA26" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="AB26" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AC26" s="17" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="27" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="31">
-        <v>0</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="E27" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="F27" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="G27" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="H27" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="I27" s="18" t="s">
-        <v>361</v>
-      </c>
-      <c r="J27" s="18" t="s">
-        <v>361</v>
-      </c>
-      <c r="K27" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="L27" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="M27" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="N27" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="O27" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="P27" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="Q27" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="R27" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="S27" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="T27" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="U27" s="18" t="s">
-        <v>364</v>
-      </c>
-      <c r="V27" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="W27" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="X27" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="Y27" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="Z27" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="AA27" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="AB27" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="AC27" s="19" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="28" spans="2:29" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="34"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22"/>
-      <c r="O28" s="22"/>
-      <c r="P28" s="22"/>
-      <c r="Q28" s="22"/>
-      <c r="R28" s="22"/>
-      <c r="S28" s="22"/>
-      <c r="T28" s="22"/>
-      <c r="U28" s="22"/>
-      <c r="V28" s="22"/>
-      <c r="W28" s="22"/>
-      <c r="X28" s="22"/>
-      <c r="Y28" s="22"/>
-      <c r="Z28" s="22"/>
-      <c r="AA28" s="22"/>
-      <c r="AB28" s="22"/>
-      <c r="AC28" s="22"/>
-    </row>
-    <row r="30" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B30" s="33" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="31" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="G32" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="H32" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="I32" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="J32" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="K32" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="L32" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="M32" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="N32" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="O32" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="P32" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q32" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="R32" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="S32" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="T32" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="U32" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="V32" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="W32" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="X32" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y32" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z32" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA32" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB32" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC32" s="26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="2:29" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" s="29">
-        <v>0</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="F33" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="G33" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="H33" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="I33" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="J33" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="K33" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="L33" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="M33" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="N33" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="O33" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="P33" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q33" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="R33" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="S33" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="T33" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="U33" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="V33" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="W33" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="X33" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y33" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z33" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="AA33" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB33" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC33" s="17" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="34" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B34" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="30">
-        <v>0</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="G34" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="H34" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="I34" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="J34" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="K34" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="L34" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="M34" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="N34" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="O34" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="P34" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q34" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="R34" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="S34" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="T34" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="U34" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="V34" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="W34" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="X34" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y34" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z34" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA34" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB34" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC34" s="17" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="35" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B35" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="30">
-        <v>0</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="F35" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="G35" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="H35" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="I35" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="J35" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="K35" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="L35" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="M35" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="N35" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="O35" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="P35" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q35" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="R35" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="S35" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="T35" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="U35" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="V35" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="W35" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="X35" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y35" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Z35" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA35" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB35" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC35" s="17" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="36" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B36" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" s="30">
-        <v>0</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="F36" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="G36" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="H36" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="I36" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="J36" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="K36" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="L36" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="M36" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="N36" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="O36" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="P36" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q36" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="R36" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="S36" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="T36" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="U36" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="V36" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="W36" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="X36" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y36" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z36" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA36" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB36" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC36" s="17" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="37" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="C37" s="31">
-        <v>0</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="F37" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="G37" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="H37" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="I37" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="J37" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="K37" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="L37" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="M37" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="N37" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O37" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="P37" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q37" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="R37" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="S37" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="T37" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="U37" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="V37" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="W37" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="X37" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y37" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z37" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA37" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB37" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC37" s="19" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="38" spans="2:29" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="34"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="22"/>
-      <c r="J38" s="22"/>
-      <c r="K38" s="22"/>
-      <c r="L38" s="22"/>
-      <c r="M38" s="22"/>
-      <c r="N38" s="22"/>
-      <c r="O38" s="22"/>
-      <c r="P38" s="22"/>
-      <c r="Q38" s="22"/>
-      <c r="R38" s="22"/>
-      <c r="S38" s="22"/>
-      <c r="T38" s="22"/>
-      <c r="U38" s="22"/>
-      <c r="V38" s="22"/>
-      <c r="W38" s="22"/>
-      <c r="X38" s="22"/>
-      <c r="Y38" s="22"/>
-      <c r="Z38" s="22"/>
-      <c r="AA38" s="22"/>
-      <c r="AB38" s="22"/>
-      <c r="AC38" s="22"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="37" stopIfTrue="1" operator="containsText" id="{5246D39B-3674-442B-A0B2-5B2C105B4832}">
-            <xm:f>NOT(ISERROR(SEARCH("++",A3)))</xm:f>
-            <xm:f>"++"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="9" tint="-0.499984740745262"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="38" stopIfTrue="1" operator="containsText" id="{49BC0916-4902-4164-9F1E-E0D19804A18D}">
-            <xm:f>NOT(ISERROR(SEARCH("+",A3)))</xm:f>
-            <xm:f>"+"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="9" tint="0.39994506668294322"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="39" stopIfTrue="1" operator="containsText" id="{6F80F022-9350-4B93-878B-5E90592F274E}">
-            <xm:f>NOT(ISERROR(SEARCH("^",A3)))</xm:f>
-            <xm:f>"^"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="9" tint="0.79998168889431442"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="40" stopIfTrue="1" operator="containsText" id="{67808645-64B8-4852-AE16-5847A12F495C}">
-            <xm:f>NOT(ISERROR(SEARCH("--",A3)))</xm:f>
-            <xm:f>"--"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFC00000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="41" stopIfTrue="1" operator="containsText" id="{7A0B4A0E-CB7F-4AF2-9CA2-90494E28A72E}">
-            <xm:f>NOT(ISERROR(SEARCH("-",A3)))</xm:f>
-            <xm:f>"-"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="5" tint="0.39994506668294322"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="42" stopIfTrue="1" operator="containsText" id="{D21E81F6-9F90-4695-87F4-912BF8BE1D78}">
-            <xm:f>NOT(ISERROR(SEARCH("v",A3)))</xm:f>
-            <xm:f>"v"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="5" tint="0.79998168889431442"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>A3:AD8 AG3:XFD8</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="13" stopIfTrue="1" operator="containsText" id="{4A8FE886-6918-440E-81B8-442AAB2E77AC}">
-            <xm:f>NOT(ISERROR(SEARCH("++",B13)))</xm:f>
-            <xm:f>"++"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="9" tint="-0.499984740745262"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="14" stopIfTrue="1" operator="containsText" id="{8CFE469A-B0C1-4FF1-A1A5-9ADF9EC37004}">
-            <xm:f>NOT(ISERROR(SEARCH("+",B13)))</xm:f>
-            <xm:f>"+"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="9" tint="0.39994506668294322"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="15" stopIfTrue="1" operator="containsText" id="{6579E2CA-F117-46A3-9341-C8B474F53E8B}">
-            <xm:f>NOT(ISERROR(SEARCH("^",B13)))</xm:f>
-            <xm:f>"^"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="9" tint="0.79998168889431442"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="16" stopIfTrue="1" operator="containsText" id="{E974AAB0-0317-4C68-9657-1057B8F5ECA6}">
-            <xm:f>NOT(ISERROR(SEARCH("--",B13)))</xm:f>
-            <xm:f>"--"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFC00000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="17" stopIfTrue="1" operator="containsText" id="{D2812EE7-C705-41D1-808D-0880013662BC}">
-            <xm:f>NOT(ISERROR(SEARCH("-",B13)))</xm:f>
-            <xm:f>"-"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="5" tint="0.39994506668294322"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="18" stopIfTrue="1" operator="containsText" id="{964C003D-5E8A-4D67-ABCF-648EA68E5F83}">
-            <xm:f>NOT(ISERROR(SEARCH("v",B13)))</xm:f>
-            <xm:f>"v"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="5" tint="0.79998168889431442"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>B13:AD18</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="7" stopIfTrue="1" operator="containsText" id="{88E01DEB-20C9-4C60-9948-DB5AC94B9C52}">
-            <xm:f>NOT(ISERROR(SEARCH("++",B22)))</xm:f>
-            <xm:f>"++"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="9" tint="-0.499984740745262"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="8" stopIfTrue="1" operator="containsText" id="{02203D4B-4A64-4024-8D9C-15F016DD85EF}">
-            <xm:f>NOT(ISERROR(SEARCH("+",B22)))</xm:f>
-            <xm:f>"+"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="9" tint="0.39994506668294322"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="9" stopIfTrue="1" operator="containsText" id="{E9080681-65C4-4651-A65D-7A6E61EC4D76}">
-            <xm:f>NOT(ISERROR(SEARCH("^",B22)))</xm:f>
-            <xm:f>"^"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="9" tint="0.79998168889431442"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="10" stopIfTrue="1" operator="containsText" id="{FDC2D42A-4471-40EC-8221-4933ABD07FB7}">
-            <xm:f>NOT(ISERROR(SEARCH("--",B22)))</xm:f>
-            <xm:f>"--"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFC00000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="11" stopIfTrue="1" operator="containsText" id="{C7EB87B2-E154-48F2-B38E-E1F6813427B8}">
-            <xm:f>NOT(ISERROR(SEARCH("-",B22)))</xm:f>
-            <xm:f>"-"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="5" tint="0.39994506668294322"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="12" stopIfTrue="1" operator="containsText" id="{AF68DCAF-938A-40F8-93FD-207499583064}">
-            <xm:f>NOT(ISERROR(SEARCH("v",B22)))</xm:f>
-            <xm:f>"v"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="5" tint="0.79998168889431442"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>B22:AC27</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="1" stopIfTrue="1" operator="containsText" id="{07198B97-AE27-4A85-BE95-2D335D19C43B}">
-            <xm:f>NOT(ISERROR(SEARCH("++",B32)))</xm:f>
-            <xm:f>"++"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="9" tint="-0.499984740745262"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="2" stopIfTrue="1" operator="containsText" id="{C3112018-6BAA-4D9D-8183-B04AFF23FB47}">
-            <xm:f>NOT(ISERROR(SEARCH("+",B32)))</xm:f>
-            <xm:f>"+"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="9" tint="0.39994506668294322"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="3" stopIfTrue="1" operator="containsText" id="{BA6C5844-3A3B-4EE2-9571-17C6D755781B}">
-            <xm:f>NOT(ISERROR(SEARCH("^",B32)))</xm:f>
-            <xm:f>"^"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="9" tint="0.79998168889431442"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="4" stopIfTrue="1" operator="containsText" id="{F76D2C6B-258B-49D1-963C-52C483AE06B0}">
-            <xm:f>NOT(ISERROR(SEARCH("--",B32)))</xm:f>
-            <xm:f>"--"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFC00000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="5" stopIfTrue="1" operator="containsText" id="{4FCF95D2-D346-4D0C-BC0F-A562C99447D2}">
-            <xm:f>NOT(ISERROR(SEARCH("-",B32)))</xm:f>
-            <xm:f>"-"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="5" tint="0.39994506668294322"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="6" stopIfTrue="1" operator="containsText" id="{66F59452-D57D-44E9-A2EB-EFF2E658F73C}">
-            <xm:f>NOT(ISERROR(SEARCH("v",B32)))</xm:f>
-            <xm:f>"v"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="5" tint="0.79998168889431442"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>B32:AC37</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added WordInPositionInLine to Experiments. Minor content changes in web pages.
</commit_message>
<xml_diff>
--- a/resources/analysis/char distribution/Character Distribution.xlsx
+++ b/resources/analysis/char distribution/Character Distribution.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\mzatt\Projects\Git - v4j\resources\analysis\char distribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2E1EDC-0B97-4BA4-9D24-9EF0218CD65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F53AB6A-0B5A-4228-B405-C4D466074E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10575" yWindow="15" windowWidth="15630" windowHeight="15585" tabRatio="806" activeTab="2" xr2:uid="{ECC3CD32-09AE-4AED-9EE9-BD1FB4BEAB7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="806" xr2:uid="{ECC3CD32-09AE-4AED-9EE9-BD1FB4BEAB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Compact" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1722" uniqueCount="624">
   <si>
     <t>Transcription     : AUGMENTED</t>
   </si>
@@ -2002,6 +2002,12 @@
   </si>
   <si>
     <t>? (0 / 1019) (0.00% / 0.08%)</t>
+  </si>
+  <si>
+    <t>Completed.</t>
+  </si>
+  <si>
+    <t>[ Last letter in a line  ]</t>
   </si>
 </sst>
 </file>
@@ -3058,8 +3064,8 @@
   </sheetPr>
   <dimension ref="A1:AI58"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M53" sqref="M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6926,10 +6932,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5676BBC-4181-4DB2-9C99-4C4C3BE5CBF3}">
-  <dimension ref="A1:AG49"/>
+  <dimension ref="A1:AG51"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="U36" sqref="U36"/>
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AK24" sqref="AK24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9221,7 +9227,7 @@
     </row>
     <row r="43" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>40</v>
+        <v>623</v>
       </c>
       <c r="B43" s="11"/>
       <c r="C43" s="10"/>
@@ -9767,6 +9773,11 @@
       </c>
       <c r="AB49" t="s">
         <v>359</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>622</v>
       </c>
     </row>
   </sheetData>
@@ -10064,7 +10075,7 @@
   </sheetPr>
   <dimension ref="A1:AJ23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>

</xml_diff>